<commit_message>
updating files and folders structure
</commit_message>
<xml_diff>
--- a/rpa-challenge.xlsx
+++ b/rpa-challenge.xlsx
@@ -461,30 +461,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Volcano Erupts in Iceland, Sending Lava Flowing Into Small Town</t>
+          <t>Trump spends Caucus Day projecting confidence, attacking rivals and thanking supporters.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jan. 13</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>The latest eruption happened along a row of volcanoes on the Reykjanes Peninsula, where a fissure opened in December, creating a river of lava.</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14xp-iceland-volcano-mbtl-threeByTwoSmallAt2X.jpg</t>
+          <t>15iowa-caucuses-trump-day-SWAP-hfqc-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -498,30 +488,20 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>How to Thrive in an Uncertain World</t>
+          <t>Ron DeSantis crosses Iowa on a freezing Caucus Day.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jan. 12</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>It’s harder than ever to predict the future. That should be a positive to embrace.</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13jackson-threeByTwoSmallAt2X-v2.jpg</t>
+          <t>15iowa-caucuses-desantis-day-lkmw-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -535,32 +515,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Why Jan. 6 Wasn’t an Insurrection</t>
+          <t>The Emmys Red Carpet Is Finally Here</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jan. 11</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Comparing the Capitol riot to the Beer Hall Putsch and the Whiskey Rebellion.</t>
+          <t>Four months later than expected, the stars have started to arrive at the 75th Emmy Awards in Los Angeles.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12douthat-newsletter-image-threeByTwoSmallAt2X.jpg</t>
+          <t>15emmys-Lakshmi-fhzq-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -572,32 +552,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Trump Dreams of Economic Disaster</t>
+          <t>The Iowans Who Are Nostalgic for Trump</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jan. 11</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Why, exactly, do so many Americans admire this guy?</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>11krugman-jwlp-threeByTwoSmallAt2X.jpg</t>
+          <t>Who hasn’t wanted a second chance in life, or the chance at a do-over?</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -609,32 +584,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>When You Return Those Pants, There’s a Price You Don’t See</t>
+          <t>My Iowa: Covering the Caucuses as a Native or a Newcomer</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jan. 10</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>The next stop for online purchases that are sent back may be the dump.</t>
+          <t>One of our reporters grew up in Iowa City and was inspired to become a journalist after witnessing the caucuses in action. Another touched down here for the first time two months ago. They compared notes.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11paul-image-threeByTwoSmallAt2X.jpg</t>
+          <t>15pol-my-iowa-top-lkzp-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -646,32 +621,32 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Biden’s Appeal to Black Voters Needs an Overhaul</t>
+          <t>The Needle Returns for the Iowa Caucus, With a Twist</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jan. 10</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>The president’s speech at Mother Emanuel was a missed opportunity.</t>
+          <t>In addition to estimating the final result, our live election model will also look at who is likeliest to take second place.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>10Blow-02-wpcl-threeByTwoSmallAt2X-v2.jpg</t>
+          <t>15pol-my-iowa-top-lkzp-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -683,32 +658,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Can Iowa Hold a Proper Caucus for Once?</t>
+          <t>The Joy of Defeat in the Iowa Caucuses</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jan. 9</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The closely-watched contest has been a hot mess for more than a decade.</t>
+          <t>Coming in second can be a win in early-state contests.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10-onpolitics-newsletter-topart-mqtl-threeByTwoSmallAt2X.jpg</t>
+          <t>15-onpolitics-newsletter-1-jcgv-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -720,32 +695,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>The Scariest Part About the Boeing 737 Max 9 Blowout</t>
+          <t>Pritzker Is Among Democrats Making Case for Biden in Iowa</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jan. 9</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What I heard wasn’t necessarily reassuring.</t>
+          <t>They argued that the future of the nation would be at risk if former President Donald J. Trump were re-elected.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10coy-newsletter-image-threeByTwoSmallAt2X.jpg</t>
+          <t>15iowa-caucuses-democrats-pritzker-gbwc-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -757,22 +732,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cost of disasters in 2023 was highest on record.</t>
+          <t>Two Young Democrats in Iowa No Longer Fear Trump</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jan. 9</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>09storms-friday-forecast-washington-vbpl-threeByTwoSmallAt2X.jpg</t>
+          <t>Jan. 14</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>They’re not persuaded that Biden would be much better.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -784,32 +764,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>The Truth About Airplane Safety</t>
+          <t>‘Oh No, They’re Both Gone’: Beloved Maine Fishing Shacks Tumble Into Bay</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jan. 8</t>
+          <t>Jan. 14</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>The Japan Airlines and Alaska Airlines incidents could have been much worse.</t>
+          <t>A video captured the moment when a winter storm surge knocked the last of the historic shacks, a local attraction and backdrop for paintings and photos, into Casco Bay.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>09tufekci4-threeByTwoSmallAt2X-v2.jpg</t>
+          <t>15xp-shacks-04-whtb-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">

</xml_diff>